<commit_message>
Updates: Mohale's Hoek, Mokhotlong, Berea
</commit_message>
<xml_diff>
--- a/Tablets Distribution - AS Training.xlsx
+++ b/Tablets Distribution - AS Training.xlsx
@@ -107,7 +107,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3138" uniqueCount="974">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3140" uniqueCount="975">
   <si>
     <t>Botha-Bothe</t>
   </si>
@@ -3029,6 +3029,9 @@
   </si>
   <si>
     <t>HA0JNW97</t>
+  </si>
+  <si>
+    <t>ABIA MOKATI SEBALO</t>
   </si>
 </sst>
 </file>
@@ -14084,6 +14087,18 @@
         <v>42458</v>
       </c>
     </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>974</v>
+      </c>
+      <c r="B8" t="s">
+        <v>844</v>
+      </c>
+      <c r="D8" s="39">
+        <f>DATE(2016,3,28)</f>
+        <v>42457</v>
+      </c>
+    </row>
     <row r="10" spans="1:5">
       <c r="E10" s="39"/>
     </row>

</xml_diff>